<commit_message>
Change imgeprocess folder list
</commit_message>
<xml_diff>
--- a/files/path_list.xlsx
+++ b/files/path_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\imageresize\powershell image resize BAS\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\ImageResizeModule\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0D1D79-1EDA-4EA5-83F4-CF5FACE8BE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0AD894-ADD4-4C0E-AB67-2E58A0FFC821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21495" yWindow="3480" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="include" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>C:\Temp\COW reports\</t>
+    <t>C:\Temp\#TEST IMAGES\</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refactored removing unneeded variables
</commit_message>
<xml_diff>
--- a/files/path_list.xlsx
+++ b/files/path_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwthomson\powershell_scripts\ImageResizeModule\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0AD894-ADD4-4C0E-AB67-2E58A0FFC821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866C3F57-2247-48A3-9FE9-8333BF705E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21495" yWindow="3480" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10005" yWindow="4920" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="include" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>path</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>C:\Temp\#TEST IMAGES\</t>
+  </si>
+  <si>
+    <t>C:\Temp\#TEST IMAGES\folder 1</t>
   </si>
 </sst>
 </file>
@@ -357,8 +360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,15 +393,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9BFF8-B01E-40C0-BF74-7EE0C47B4272}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,6 +412,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>